<commit_message>
added excel generation, base xml and excel split of cases with array
</commit_message>
<xml_diff>
--- a/excel/posible nuevo excel base.xlsx
+++ b/excel/posible nuevo excel base.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Documents\projects\WPG\nl protocol\NL protocol Python Geerator\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView minimized="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="175">
   <si>
     <t>L1</t>
   </si>
@@ -37,9 +37,6 @@
     <t>L5</t>
   </si>
   <si>
-    <t>path</t>
-  </si>
-  <si>
     <t>Default Values</t>
   </si>
   <si>
@@ -487,9 +484,6 @@
     <t>correct net area</t>
   </si>
   <si>
-    <t>supplier, reciver, sender, operator</t>
-  </si>
-  <si>
     <t>net areas</t>
   </si>
   <si>
@@ -502,9 +496,6 @@
     <t>water</t>
   </si>
   <si>
-    <t>correct net area2, cod2</t>
-  </si>
-  <si>
     <t>2021-03-03T22:00:00Z</t>
   </si>
   <si>
@@ -533,6 +524,27 @@
   </si>
   <si>
     <t>de donde saca los valores de time series (extrahourDLS_day,lesshourDLS_day,normal_day,etc)</t>
+  </si>
+  <si>
+    <t>struct</t>
+  </si>
+  <si>
+    <t>2021-03-04T22:00:00Z</t>
+  </si>
+  <si>
+    <t>cod3</t>
+  </si>
+  <si>
+    <t>sender belen</t>
+  </si>
+  <si>
+    <t>belen sender</t>
+  </si>
+  <si>
+    <t>supplier, reciver, sender, operator, sender belen</t>
+  </si>
+  <si>
+    <t>XML ELEMENT PATH</t>
   </si>
 </sst>
 </file>
@@ -556,7 +568,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -566,6 +578,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -610,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -623,6 +641,8 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -929,16 +949,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F42" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" topLeftCell="F45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56:H72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="107" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="107.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="37.28515625" customWidth="1"/>
+    <col min="1" max="2" width="3.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="83.85546875" customWidth="1"/>
+    <col min="7" max="7" width="85.7109375" customWidth="1"/>
+    <col min="8" max="8" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -958,36 +982,36 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H2" s="2" t="str">
         <f t="shared" ref="H2:H11" si="0">G2</f>
@@ -1000,13 +1024,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H3" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1019,13 +1043,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1038,17 +1062,16 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="H5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>2021-03-03T22:00:00Z</v>
+        <v>158</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1057,13 +1080,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1076,13 +1099,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1093,34 +1116,34 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="H8" s="2" t="str">
+    <row r="8" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H8" s="9" t="str">
         <f t="shared" si="0"/>
         <v>NLPROTOC-OLER-ROR0-0000-000000000000</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H9" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1133,13 +1156,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1152,13 +1175,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H11" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1171,13 +1194,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H12" s="2" t="str">
         <f t="shared" ref="H12:H50" si="1">G12</f>
@@ -1190,13 +1213,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H13" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1209,13 +1232,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H14" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1228,13 +1251,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H15" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1247,13 +1270,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H16" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1266,13 +1289,13 @@
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H17" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1285,13 +1308,13 @@
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H18" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1304,13 +1327,13 @@
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H19" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1323,13 +1346,13 @@
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H20" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1342,13 +1365,13 @@
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H21" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1361,13 +1384,13 @@
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H22" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1380,13 +1403,13 @@
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H23" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1399,13 +1422,13 @@
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H24" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1418,13 +1441,13 @@
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H25" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1437,13 +1460,13 @@
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H26" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1456,13 +1479,13 @@
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H27" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1473,34 +1496,34 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="H28" s="2" t="str">
+    <row r="28" spans="3:12" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H28" s="9" t="str">
         <f t="shared" si="1"/>
         <v>NLPROTOC-OLER-ROR0-0000-000000000000</v>
       </c>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H29" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1513,13 +1536,13 @@
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H30" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1532,13 +1555,13 @@
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H31" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1551,13 +1574,13 @@
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H32" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1570,13 +1593,13 @@
     </row>
     <row r="33" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H33" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1589,13 +1612,13 @@
     </row>
     <row r="34" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H34" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1608,13 +1631,13 @@
     </row>
     <row r="35" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H35" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1627,13 +1650,13 @@
     </row>
     <row r="36" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H36" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1646,13 +1669,13 @@
     </row>
     <row r="37" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H37" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1665,13 +1688,13 @@
     </row>
     <row r="38" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H38" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1684,13 +1707,13 @@
     </row>
     <row r="39" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H39" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1703,13 +1726,13 @@
     </row>
     <row r="40" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H40" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1722,13 +1745,13 @@
     </row>
     <row r="41" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H41" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1741,16 +1764,16 @@
     </row>
     <row r="42" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -1759,13 +1782,13 @@
     </row>
     <row r="43" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H43" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1778,13 +1801,13 @@
     </row>
     <row r="44" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H44" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1797,13 +1820,13 @@
     </row>
     <row r="45" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H45" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1816,13 +1839,13 @@
     </row>
     <row r="46" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H46" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1835,13 +1858,13 @@
     </row>
     <row r="47" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H47" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1854,13 +1877,13 @@
     </row>
     <row r="48" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H48" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1873,10 +1896,10 @@
     </row>
     <row r="49" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -1887,13 +1910,13 @@
     </row>
     <row r="50" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H50" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1942,7 +1965,7 @@
     </row>
     <row r="55" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F55" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
@@ -1953,13 +1976,13 @@
     </row>
     <row r="56" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F56" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
@@ -1968,14 +1991,14 @@
     </row>
     <row r="57" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F57" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G57" s="2" t="str">
         <f>CONCATENATE("MeasurementSeriesNotification_ErrorCode_",G59,"_col_nombredecol")</f>
         <v>MeasurementSeriesNotification_ErrorCode_0_col_nombredecol</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
@@ -1984,13 +2007,13 @@
     </row>
     <row r="58" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F58" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
@@ -1999,13 +2022,13 @@
     </row>
     <row r="59" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F59" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G59" s="2">
         <v>0</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
@@ -2014,7 +2037,7 @@
     </row>
     <row r="60" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F60" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G60" s="2" t="str">
         <f>G$8</f>
@@ -2031,7 +2054,7 @@
     </row>
     <row r="61" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F61" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G61" s="2" t="str">
         <f>G$37</f>
@@ -2048,7 +2071,7 @@
     </row>
     <row r="62" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F62" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G62" s="2" t="str">
         <f>G$38</f>
@@ -2065,7 +2088,7 @@
     </row>
     <row r="63" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F63" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G63" s="6" t="str">
         <f>G14</f>
@@ -2082,7 +2105,7 @@
     </row>
     <row r="64" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F64" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G64" s="2" t="str">
         <f>G31</f>
@@ -2099,7 +2122,7 @@
     </row>
     <row r="65" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F65" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G65" s="2" t="str">
         <f>G42</f>
@@ -2116,13 +2139,13 @@
     </row>
     <row r="66" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F66" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
@@ -2130,7 +2153,9 @@
       <c r="L66" s="2"/>
     </row>
     <row r="67" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F67" s="2"/>
+      <c r="F67" s="2" t="s">
+        <v>168</v>
+      </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
@@ -2140,14 +2165,14 @@
     </row>
     <row r="68" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F68" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="H68" s="2" t="str">
         <f>G68</f>
-        <v>supplier, reciver, sender, operator</v>
+        <v>supplier, reciver, sender, operator, sender belen</v>
       </c>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
@@ -2156,14 +2181,14 @@
     </row>
     <row r="69" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F69" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="H69" s="2" t="str">
         <f>G69</f>
-        <v>correct net area2, cod2</v>
+        <v>cod3</v>
       </c>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
@@ -2172,7 +2197,7 @@
     </row>
     <row r="70" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F70" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
@@ -2183,7 +2208,7 @@
     </row>
     <row r="71" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F71" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -2194,7 +2219,7 @@
     </row>
     <row r="72" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F72" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
@@ -2210,10 +2235,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2228,49 +2253,55 @@
     <col min="12" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="F2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="B3" s="3">
         <v>8716948001031</v>
@@ -2287,56 +2318,68 @@
       <c r="F3" s="3">
         <v>8716948001024</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="4">
+        <v>123123132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>138</v>
-      </c>
       <c r="C4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>142</v>
-      </c>
       <c r="F4" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="B8" s="3">
         <v>8.7169210000000998E+17</v>
@@ -2347,24 +2390,30 @@
       <c r="D8" s="3">
         <v>8.7169210000000998E+17</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="3">
+        <v>8.7169210000000998E+17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B10" s="3">
         <v>8716948001024</v>
@@ -2375,19 +2424,23 @@
       <c r="D10" s="3">
         <v>8716948001024</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>